<commit_message>
Edit test excel files
</commit_message>
<xml_diff>
--- a/Test_data/box_set_01.xlsx
+++ b/Test_data/box_set_01.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\First-AP\Desktop\Homework\4th Year\2nd term\Container_loding\project\Test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE1FB782-0F9A-4263-977C-0773BE19790C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B519724-0D8C-44D1-8F63-C86C73EAB5BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0F278F22-566D-45EB-B0E9-07BA93203C9F}"/>
   </bookViews>
@@ -96,10 +96,10 @@
     <t>CM</t>
   </si>
   <si>
-    <t>IN</t>
-  </si>
-  <si>
-    <t>in</t>
+    <t>inch</t>
+  </si>
+  <si>
+    <t>INch</t>
   </si>
 </sst>
 </file>
@@ -472,7 +472,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.6" x14ac:dyDescent="0.3"/>
@@ -760,7 +760,7 @@
         <v>6</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -800,7 +800,7 @@
         <v>6</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>